<commit_message>
match by pmid or overlap of accession, if no match then title
</commit_message>
<xml_diff>
--- a/Pubmed/Nipah/ReferenceSummary_PubMed_Missing_Jan31.xlsx
+++ b/Pubmed/Nipah/ReferenceSummary_PubMed_Missing_Jan31.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaimingtao/Library/CloudStorage/Dropbox/Shared/___SystematicReviewsAI/Nipah/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E961EFF-AEDD-464F-89AA-9D61E3B0FF33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC00B2B-2B8C-664E-8933-39ABF909B8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9520" yWindow="5320" windowWidth="37760" windowHeight="19780" xr2:uid="{3031CDAD-EDE9-504F-A9EA-0D1529922A9B}"/>
+    <workbookView xWindow="640" yWindow="1820" windowWidth="37760" windowHeight="19780" xr2:uid="{3031CDAD-EDE9-504F-A9EA-0D1529922A9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -173,9 +173,6 @@
     <t>P, N</t>
   </si>
   <si>
-    <t>2002 to 2008</t>
-  </si>
-  <si>
     <t>Thailand</t>
   </si>
   <si>
@@ -195,6 +192,9 @@
   </si>
   <si>
     <t>N, P, M, F, G, L</t>
+  </si>
+  <si>
+    <t>2002-2008</t>
   </si>
 </sst>
 </file>
@@ -666,7 +666,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R14" sqref="R14"/>
+      <selection pane="bottomLeft" activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -835,13 +835,13 @@
         <v>38</v>
       </c>
       <c r="P3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>25</v>
@@ -850,10 +850,10 @@
         <v>24</v>
       </c>
       <c r="U3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="48" x14ac:dyDescent="0.2">
@@ -876,7 +876,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>38</v>
@@ -885,7 +885,7 @@
         <v>2009</v>
       </c>
       <c r="Q4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>25</v>
@@ -897,7 +897,7 @@
         <v>42</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>